<commit_message>
java script ended and js in browser begins
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>action</t>
   </si>
@@ -31,9 +36,6 @@
     <t>java script</t>
   </si>
   <si>
-    <t>10h 30m</t>
-  </si>
-  <si>
     <t>end</t>
   </si>
   <si>
@@ -41,13 +43,15 @@
   </si>
   <si>
     <t>_</t>
+  </si>
+  <si>
+    <t>js in browser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,28 +95,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -123,10 +130,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -164,71 +171,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -256,7 +263,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -279,11 +286,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -292,13 +299,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -308,7 +315,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -317,7 +324,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -326,7 +333,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -334,10 +341,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -406,19 +413,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,32 +441,46 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
js in browser ET 0h 27m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>action</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>js in browser</t>
+  </si>
+  <si>
+    <t>0h 27m</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,11 +448,11 @@
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
+      <c r="B2" s="1">
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
html css ET 0h 5m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>action</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>0h 27m</t>
+  </si>
+  <si>
+    <t>html css</t>
+  </si>
+  <si>
+    <t>0h 5m</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,15 +480,29 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
js br ET 1h 2m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -48,13 +48,13 @@
     <t>js in browser</t>
   </si>
   <si>
-    <t>0h 27m</t>
-  </si>
-  <si>
     <t>html css</t>
   </si>
   <si>
     <t>0h 5m</t>
+  </si>
+  <si>
+    <t>1h 2m</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -480,13 +480,13 @@
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
jsbr ET 0h 22m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -51,10 +51,10 @@
     <t>html css</t>
   </si>
   <si>
-    <t>0h 5m</t>
-  </si>
-  <si>
     <t>1h 2m</t>
+  </si>
+  <si>
+    <t>0h 22m</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -486,7 +486,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
parts error was resolved
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -424,8 +424,8 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
c++ ET 0h 35m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>action</t>
   </si>
@@ -33,34 +28,38 @@
     <t>part</t>
   </si>
   <si>
+    <t>js in browser</t>
+  </si>
+  <si>
+    <t>1h 2m</t>
+  </si>
+  <si>
+    <t>c++</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>0h 35m</t>
+  </si>
+  <si>
+    <t>html css</t>
+  </si>
+  <si>
+    <t>0h 22m</t>
+  </si>
+  <si>
     <t>java script</t>
   </si>
   <si>
     <t>end</t>
-  </si>
-  <si>
-    <t>c++</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>js in browser</t>
-  </si>
-  <si>
-    <t>html css</t>
-  </si>
-  <si>
-    <t>1h 2m</t>
-  </si>
-  <si>
-    <t>0h 22m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,7 +70,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -104,31 +103,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -139,10 +135,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -180,71 +176,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -272,7 +268,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -295,11 +291,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -308,13 +304,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -324,7 +320,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -333,7 +329,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -342,7 +338,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -350,10 +346,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -424,23 +420,21 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -450,57 +444,57 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
-        <v>0</v>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
js br 1h 19m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -31,7 +31,7 @@
     <t>js in browser</t>
   </si>
   <si>
-    <t>1h 2m</t>
+    <t>1h 19m</t>
   </si>
   <si>
     <t>c++</t>
@@ -426,7 +426,7 @@
   <cols>
     <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -437,7 +437,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -451,7 +451,7 @@
       <c r="B2" s="2">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="2">
@@ -465,7 +465,7 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2">
@@ -479,7 +479,7 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="2">
@@ -493,7 +493,7 @@
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="2">

</xml_diff>

<commit_message>
jsbr ET 1h 55m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -31,9 +36,6 @@
     <t>js in browser</t>
   </si>
   <si>
-    <t>1h 19m</t>
-  </si>
-  <si>
     <t>c++</t>
   </si>
   <si>
@@ -53,13 +55,15 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>1h 55m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,28 +107,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -135,10 +142,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -176,71 +183,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -268,7 +275,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -291,11 +298,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -304,13 +311,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -320,7 +327,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -329,7 +336,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -338,7 +345,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -346,10 +353,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -420,17 +427,19 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -452,49 +461,49 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
c++ ET 1h 27m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -36,13 +31,16 @@
     <t>js in browser</t>
   </si>
   <si>
+    <t>1h 55m</t>
+  </si>
+  <si>
     <t>c++</t>
   </si>
   <si>
     <t>_</t>
   </si>
   <si>
-    <t>1h 2m</t>
+    <t>1h 27m</t>
   </si>
   <si>
     <t>html css</t>
@@ -55,15 +53,13 @@
   </si>
   <si>
     <t>end</t>
-  </si>
-  <si>
-    <t>1h 55m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,31 +103,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -142,10 +135,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -183,71 +176,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -275,7 +268,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -298,11 +291,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -311,13 +304,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -327,7 +320,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -336,7 +329,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -345,7 +338,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -353,10 +346,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -427,19 +420,17 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -461,49 +452,49 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
jsbr ET 2h 28m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -31,9 +36,6 @@
     <t>js in browser</t>
   </si>
   <si>
-    <t>1h 55m</t>
-  </si>
-  <si>
     <t>c++</t>
   </si>
   <si>
@@ -53,13 +55,15 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>2h 28m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,28 +107,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -135,10 +142,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -176,71 +183,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -268,7 +275,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -291,11 +298,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -304,13 +311,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -320,7 +327,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -329,7 +336,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -338,7 +345,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -346,10 +353,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -420,17 +427,19 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -452,49 +461,49 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
jsbr ET 2h 42m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -57,7 +57,7 @@
     <t>end</t>
   </si>
   <si>
-    <t>2h 28m</t>
+    <t>2h 42m</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
jsbr ET 2h 57m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -36,6 +31,9 @@
     <t>js in browser</t>
   </si>
   <si>
+    <t>2h 57m</t>
+  </si>
+  <si>
     <t>c++</t>
   </si>
   <si>
@@ -55,15 +53,13 @@
   </si>
   <si>
     <t>end</t>
-  </si>
-  <si>
-    <t>2h 42m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,31 +103,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -142,10 +135,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -183,71 +176,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -275,7 +268,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -298,11 +291,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -311,13 +304,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -327,7 +320,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -336,7 +329,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -345,7 +338,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -353,10 +346,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -427,19 +420,17 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -461,49 +452,49 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
web design 0h 59m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -43,23 +48,22 @@
     <t>1h 27m</t>
   </si>
   <si>
-    <t>html css</t>
-  </si>
-  <si>
-    <t>0h 22m</t>
-  </si>
-  <si>
     <t>java script</t>
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>0h 59m</t>
+  </si>
+  <si>
+    <t>web design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,28 +107,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -135,10 +142,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -176,71 +183,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -268,7 +275,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -291,11 +298,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -304,13 +311,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -320,7 +327,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -329,7 +336,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -338,7 +345,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -346,10 +353,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -420,17 +427,19 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -458,7 +467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -472,29 +481,29 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
jsbr ET 3h 23m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -36,9 +36,6 @@
     <t>js in browser</t>
   </si>
   <si>
-    <t>2h 57m</t>
-  </si>
-  <si>
     <t>c++</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>web design</t>
+  </si>
+  <si>
+    <t>3h 23m</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -469,13 +469,13 @@
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
@@ -483,13 +483,13 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
@@ -497,13 +497,13 @@
     </row>
     <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
web design 1h 2m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -51,13 +51,13 @@
     <t>end</t>
   </si>
   <si>
-    <t>0h 59m</t>
-  </si>
-  <si>
     <t>web design</t>
   </si>
   <si>
     <t>3h 23m</t>
+  </si>
+  <si>
+    <t>1h 02m</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -483,13 +483,13 @@
     </row>
     <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
jsbr ET 4h 33m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -31,9 +36,6 @@
     <t>js in browser</t>
   </si>
   <si>
-    <t>4h 3m</t>
-  </si>
-  <si>
     <t>c++</t>
   </si>
   <si>
@@ -53,18 +55,20 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>4h 33m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -103,28 +107,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -135,10 +142,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -176,71 +183,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -268,7 +275,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -291,11 +298,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -304,13 +311,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -320,7 +327,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -329,7 +336,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -338,7 +345,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -346,10 +353,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -420,17 +427,19 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="27.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -452,49 +461,49 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
jsbr ET 3h 35m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perfect\Desktop\actional\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -36,34 +31,35 @@
     <t>js in browser</t>
   </si>
   <si>
+    <t>3h 35m</t>
+  </si>
+  <si>
     <t>c++</t>
   </si>
   <si>
     <t>_</t>
   </si>
   <si>
+    <t>2h 20m</t>
+  </si>
+  <si>
+    <t>web design</t>
+  </si>
+  <si>
+    <t>1h 02m</t>
+  </si>
+  <si>
     <t>java script</t>
   </si>
   <si>
     <t>end</t>
-  </si>
-  <si>
-    <t>web design</t>
-  </si>
-  <si>
-    <t>3h 23m</t>
-  </si>
-  <si>
-    <t>1h 02m</t>
-  </si>
-  <si>
-    <t>2h 20m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,31 +103,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -142,10 +135,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -183,71 +176,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -275,7 +268,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -298,11 +291,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -311,13 +304,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -327,7 +320,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -336,7 +329,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -345,7 +338,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -353,10 +346,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -427,19 +420,17 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="3" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="21.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="24.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -461,49 +452,49 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
jsbr ET 7h 50m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -57,7 +57,7 @@
     <t>end</t>
   </si>
   <si>
-    <t>4h 33m</t>
+    <t>7h 50m</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
c++ RT 2h 11m p3
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>action</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>7h 50m</t>
+  </si>
+  <si>
+    <t>2h 11m p3</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -471,8 +474,8 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
-        <v>0</v>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
jsbr ET 1h 13m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>action</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>2h 11m p3</t>
+  </si>
+  <si>
+    <t>1h 13m</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -461,10 +464,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
jsbr ET 1h 29m
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -60,7 +60,7 @@
     <t>2h 11m p3</t>
   </si>
   <si>
-    <t>1h 13m</t>
+    <t>1h 29m</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
jsbr ET part2 ended
</commit_message>
<xml_diff>
--- a/actional.xlsx
+++ b/actional.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>action</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>2h 11m p3</t>
-  </si>
-  <si>
-    <t>1h 55m</t>
   </si>
 </sst>
 </file>
@@ -431,7 +428,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -464,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>

</xml_diff>